<commit_message>
Now including formal-only labor.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/SUN/SUN Data.xlsx
+++ b/data/Excel Workbooks/SUN/SUN Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="0" windowWidth="25040" windowHeight="17000" tabRatio="500"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="223">
   <si>
     <t>Year</t>
   </si>
@@ -691,6 +691,12 @@
   </si>
   <si>
     <t>iYear</t>
+  </si>
+  <si>
+    <t>iL_ForAndInfor</t>
+  </si>
+  <si>
+    <t>iL_For</t>
   </si>
 </sst>
 </file>
@@ -968,10 +974,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1221,7 +1233,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="29">
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1233,6 +1245,9 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1243,6 +1258,9 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1672,15 +1690,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B69"/>
+      <selection activeCell="G2" sqref="G2:G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1694,22 +1712,28 @@
         <v>212</v>
       </c>
       <c r="E1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" t="s">
         <v>213</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>214</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>215</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>217</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1946</v>
       </c>
@@ -1731,17 +1755,24 @@
       <c r="F2" t="s">
         <v>216</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="str">
+        <f>F2</f>
+        <v>NA</v>
+      </c>
+      <c r="H2" t="s">
         <v>216</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" t="s">
         <v>219</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1947</v>
       </c>
@@ -1763,17 +1794,24 @@
       <c r="F3" t="s">
         <v>216</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G66" si="1">F3</f>
+        <v>NA</v>
+      </c>
+      <c r="H3" t="s">
         <v>216</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J3" t="s">
         <v>219</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1948</v>
       </c>
@@ -1795,17 +1833,24 @@
       <c r="F4" t="s">
         <v>216</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H4" t="s">
         <v>216</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>216</v>
+      </c>
+      <c r="J4" t="s">
         <v>219</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1949</v>
       </c>
@@ -1827,17 +1872,24 @@
       <c r="F5" t="s">
         <v>216</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H5" t="s">
         <v>216</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5" t="s">
         <v>219</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1950</v>
       </c>
@@ -1859,17 +1911,24 @@
       <c r="F6" t="s">
         <v>216</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H6" t="s">
         <v>216</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J6" t="s">
         <v>219</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1951</v>
       </c>
@@ -1891,17 +1950,24 @@
       <c r="F7" t="s">
         <v>216</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H7" t="s">
         <v>216</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J7" t="s">
         <v>219</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1952</v>
       </c>
@@ -1923,17 +1989,24 @@
       <c r="F8" t="s">
         <v>216</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H8" t="s">
         <v>216</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
+        <v>216</v>
+      </c>
+      <c r="J8" t="s">
         <v>219</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>1953</v>
       </c>
@@ -1955,17 +2028,24 @@
       <c r="F9" t="s">
         <v>216</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H9" t="s">
         <v>216</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
+        <v>216</v>
+      </c>
+      <c r="J9" t="s">
         <v>219</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>1954</v>
       </c>
@@ -1987,17 +2067,24 @@
       <c r="F10" t="s">
         <v>216</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H10" t="s">
         <v>216</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
+        <v>216</v>
+      </c>
+      <c r="J10" t="s">
         <v>219</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>1955</v>
       </c>
@@ -2019,17 +2106,24 @@
       <c r="F11" t="s">
         <v>216</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H11" t="s">
         <v>216</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>216</v>
+      </c>
+      <c r="J11" t="s">
         <v>219</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>1956</v>
       </c>
@@ -2051,17 +2145,24 @@
       <c r="F12" t="s">
         <v>216</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H12" t="s">
         <v>216</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
+        <v>216</v>
+      </c>
+      <c r="J12" t="s">
         <v>219</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>1957</v>
       </c>
@@ -2083,17 +2184,24 @@
       <c r="F13" t="s">
         <v>216</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H13" t="s">
         <v>216</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
+        <v>216</v>
+      </c>
+      <c r="J13" t="s">
         <v>219</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>1958</v>
       </c>
@@ -2115,17 +2223,24 @@
       <c r="F14" t="s">
         <v>216</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H14" t="s">
         <v>216</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
+        <v>216</v>
+      </c>
+      <c r="J14" t="s">
         <v>219</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>1959</v>
       </c>
@@ -2147,17 +2262,24 @@
       <c r="F15" t="s">
         <v>216</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H15" t="s">
         <v>216</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>216</v>
+      </c>
+      <c r="J15" t="s">
         <v>219</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>1960</v>
       </c>
@@ -2179,17 +2301,24 @@
       <c r="F16" t="s">
         <v>216</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H16" t="s">
         <v>216</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
+        <v>216</v>
+      </c>
+      <c r="J16" t="s">
         <v>219</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>1961</v>
       </c>
@@ -2211,17 +2340,24 @@
       <c r="F17" t="s">
         <v>216</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H17" t="s">
         <v>216</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
+        <v>216</v>
+      </c>
+      <c r="J17" t="s">
         <v>219</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>1962</v>
       </c>
@@ -2243,17 +2379,24 @@
       <c r="F18" t="s">
         <v>216</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H18" t="s">
         <v>216</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
+        <v>216</v>
+      </c>
+      <c r="J18" t="s">
         <v>219</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>1963</v>
       </c>
@@ -2275,17 +2418,24 @@
       <c r="F19" t="s">
         <v>216</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H19" t="s">
         <v>216</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
+        <v>216</v>
+      </c>
+      <c r="J19" t="s">
         <v>219</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>1964</v>
       </c>
@@ -2307,17 +2457,24 @@
       <c r="F20" t="s">
         <v>216</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H20" t="s">
         <v>216</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>216</v>
+      </c>
+      <c r="J20" t="s">
         <v>219</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>1965</v>
       </c>
@@ -2339,17 +2496,24 @@
       <c r="F21" t="s">
         <v>216</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H21" t="s">
         <v>216</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
+        <v>216</v>
+      </c>
+      <c r="J21" t="s">
         <v>219</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>1966</v>
       </c>
@@ -2371,17 +2535,24 @@
       <c r="F22" t="s">
         <v>216</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H22" t="s">
         <v>216</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
+        <v>216</v>
+      </c>
+      <c r="J22" t="s">
         <v>219</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>1967</v>
       </c>
@@ -2403,17 +2574,24 @@
       <c r="F23" t="s">
         <v>216</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H23" t="s">
         <v>216</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>216</v>
+      </c>
+      <c r="J23" t="s">
         <v>219</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>1968</v>
       </c>
@@ -2435,17 +2613,24 @@
       <c r="F24" t="s">
         <v>216</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H24" t="s">
         <v>216</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
+        <v>216</v>
+      </c>
+      <c r="J24" t="s">
         <v>219</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>1969</v>
       </c>
@@ -2467,17 +2652,24 @@
       <c r="F25" t="s">
         <v>216</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="H25" t="s">
         <v>216</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
+        <v>216</v>
+      </c>
+      <c r="J25" t="s">
         <v>219</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>1970</v>
       </c>
@@ -2497,20 +2689,28 @@
         <f>'labour '!C33/'labour '!$C$36</f>
         <v>0.91028898317353013</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26">
+        <f>'labour '!B33/'labour '!$B$36</f>
+        <v>0.92333577712232928</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0.92333577712232928</v>
+      </c>
+      <c r="H26" t="s">
         <v>216</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>216</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>219</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>1971</v>
       </c>
@@ -2530,20 +2730,28 @@
         <f>'labour '!C34/'labour '!$C$36</f>
         <v>0.93703340039849192</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27">
+        <f>'labour '!B34/'labour '!$B$36</f>
+        <v>0.9445901877653603</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>0.9445901877653603</v>
+      </c>
+      <c r="H27" t="s">
         <v>216</v>
       </c>
-      <c r="G27" t="s">
+      <c r="I27" t="s">
         <v>216</v>
       </c>
-      <c r="H27" t="s">
+      <c r="J27" t="s">
         <v>219</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>1972</v>
       </c>
@@ -2563,20 +2771,28 @@
         <f>'labour '!C35/'labour '!$C$36</f>
         <v>0.95822256873969847</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28">
+        <f>'labour '!B35/'labour '!$B$36</f>
+        <v>0.96118443852064028</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0.96118443852064028</v>
+      </c>
+      <c r="H28" t="s">
         <v>216</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>216</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>219</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>1973</v>
       </c>
@@ -2597,26 +2813,34 @@
         <v>1</v>
       </c>
       <c r="F29">
+        <f>'labour '!B36/'labour '!$B$36</f>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
         <f>'Energy data'!K16/'Energy data'!$K$16</f>
         <v>1</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <f>'Energy data'!R16/'Energy data'!$R$16</f>
         <v>1</v>
       </c>
-      <c r="H29" t="s">
+      <c r="J29" t="s">
         <v>219</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>1974</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:B69" si="1">A30-$A$29</f>
+        <f t="shared" ref="B30:B69" si="2">A30-$A$29</f>
         <v>1</v>
       </c>
       <c r="C30">
@@ -2632,26 +2856,34 @@
         <v>1.0382444840804939</v>
       </c>
       <c r="F30">
+        <f>'labour '!B37/'labour '!$B$36</f>
+        <v>1.0358570789501769</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>1.0358570789501769</v>
+      </c>
+      <c r="H30">
         <f>'Energy data'!K17/'Energy data'!$K$16</f>
         <v>1.029990951006162</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <f>'Energy data'!R17/'Energy data'!$R$16</f>
         <v>1.0051975702924416</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" t="s">
         <v>219</v>
       </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>1975</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C31">
@@ -2667,26 +2899,34 @@
         <v>1.0727206861973357</v>
       </c>
       <c r="F31">
+        <f>'labour '!B38/'labour '!$B$36</f>
+        <v>1.0680120517764264</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>1.0680120517764264</v>
+      </c>
+      <c r="H31">
         <f>'Energy data'!K18/'Energy data'!$K$16</f>
         <v>1.1190589046408412</v>
       </c>
-      <c r="G31">
+      <c r="I31">
         <f>'Energy data'!R18/'Energy data'!$R$16</f>
         <v>1.0780261757154486</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>219</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>1976</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C32">
@@ -2702,26 +2942,34 @@
         <v>1.0866430331832257</v>
       </c>
       <c r="F32">
+        <f>'labour '!B39/'labour '!$B$36</f>
+        <v>1.0768993110404073</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>1.0768993110404073</v>
+      </c>
+      <c r="H32">
         <f>'Energy data'!K19/'Energy data'!$K$16</f>
         <v>1.168009652260094</v>
       </c>
-      <c r="G32">
+      <c r="I32">
         <f>'Energy data'!R19/'Energy data'!$R$16</f>
         <v>1.1149101383931368</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>219</v>
       </c>
-      <c r="I32" t="s">
+      <c r="K32" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>1977</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C33">
@@ -2737,26 +2985,34 @@
         <v>1.0788515234614313</v>
       </c>
       <c r="F33">
+        <f>'labour '!B40/'labour '!$B$36</f>
+        <v>1.0623062619489441</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>1.0623062619489441</v>
+      </c>
+      <c r="H33">
         <f>'Energy data'!K20/'Energy data'!$K$16</f>
         <v>1.1740423148188048</v>
       </c>
-      <c r="G33">
+      <c r="I33">
         <f>'Energy data'!R20/'Energy data'!$R$16</f>
         <v>1.089172772246227</v>
       </c>
-      <c r="H33" t="s">
+      <c r="J33" t="s">
         <v>219</v>
       </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>1978</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C34">
@@ -2772,26 +3028,34 @@
         <v>1.0876250373653398</v>
       </c>
       <c r="F34">
+        <f>'labour '!B41/'labour '!$B$36</f>
+        <v>1.0643549715500999</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>1.0643549715500999</v>
+      </c>
+      <c r="H34">
         <f>'Energy data'!K21/'Energy data'!$K$16</f>
         <v>1.075537553324428</v>
       </c>
-      <c r="G34">
+      <c r="I34">
         <f>'Energy data'!R21/'Energy data'!$R$16</f>
         <v>1.1509174024672801</v>
       </c>
-      <c r="H34" t="s">
+      <c r="J34" t="s">
         <v>219</v>
       </c>
-      <c r="I34" t="s">
+      <c r="K34" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>1979</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="C35">
@@ -2807,26 +3071,34 @@
         <v>1.1073602082196052</v>
       </c>
       <c r="F35">
+        <f>'labour '!B42/'labour '!$B$36</f>
+        <v>1.0791226334849746</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>1.0791226334849746</v>
+      </c>
+      <c r="H35">
         <f>'Energy data'!K22/'Energy data'!$K$16</f>
         <v>1.0948851639591504</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <f>'Energy data'!R22/'Energy data'!$R$16</f>
         <v>1.1403343978959233</v>
       </c>
-      <c r="H35" t="s">
+      <c r="J35" t="s">
         <v>219</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>1980</v>
       </c>
       <c r="B36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="C36">
@@ -2842,26 +3114,34 @@
         <v>1.1471964646370654</v>
       </c>
       <c r="F36">
+        <f>'labour '!B43/'labour '!$B$36</f>
+        <v>1.1151765261466215</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>1.1151765261466215</v>
+      </c>
+      <c r="H36">
         <f>'Energy data'!K23/'Energy data'!$K$16</f>
         <v>1.1518076442452707</v>
       </c>
-      <c r="G36">
+      <c r="I36">
         <f>'Energy data'!R23/'Energy data'!$R$16</f>
         <v>1.1834178721272464</v>
       </c>
-      <c r="H36" t="s">
+      <c r="J36" t="s">
         <v>219</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>1981</v>
       </c>
       <c r="B37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C37">
@@ -2877,26 +3157,34 @@
         <v>1.1833235328591227</v>
       </c>
       <c r="F37">
+        <f>'labour '!B44/'labour '!$B$36</f>
+        <v>1.1481994435684739</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>1.1481994435684739</v>
+      </c>
+      <c r="H37">
         <f>'Energy data'!K24/'Energy data'!$K$16</f>
         <v>1.2102382901710691</v>
       </c>
-      <c r="G37">
+      <c r="I37">
         <f>'Energy data'!R24/'Energy data'!$R$16</f>
         <v>1.2435969691276849</v>
       </c>
-      <c r="H37" t="s">
+      <c r="J37" t="s">
         <v>219</v>
       </c>
-      <c r="I37" t="s">
+      <c r="K37" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>1982</v>
       </c>
       <c r="B38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C38">
@@ -2912,26 +3200,34 @@
         <v>1.2014983241337824</v>
       </c>
       <c r="F38">
+        <f>'labour '!B45/'labour '!$B$36</f>
+        <v>1.1610506301282266</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>1.1610506301282266</v>
+      </c>
+      <c r="H38">
         <f>'Energy data'!K25/'Energy data'!$K$16</f>
         <v>1.2000689447149568</v>
       </c>
-      <c r="G38">
+      <c r="I38">
         <f>'Energy data'!R25/'Energy data'!$R$16</f>
         <v>1.1981965057298516</v>
       </c>
-      <c r="H38" t="s">
+      <c r="J38" t="s">
         <v>219</v>
       </c>
-      <c r="I38" t="s">
+      <c r="K38" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>1983</v>
       </c>
       <c r="B39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C39">
@@ -2947,26 +3243,34 @@
         <v>1.200218407432375</v>
       </c>
       <c r="F39">
+        <f>'labour '!B46/'labour '!$B$36</f>
+        <v>1.1527824606649568</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>1.1527824606649568</v>
+      </c>
+      <c r="H39">
         <f>'Energy data'!K26/'Energy data'!$K$16</f>
         <v>1.1808075149739305</v>
       </c>
-      <c r="G39">
+      <c r="I39">
         <f>'Energy data'!R26/'Energy data'!$R$16</f>
         <v>1.1678251612499218</v>
       </c>
-      <c r="H39" t="s">
+      <c r="J39" t="s">
         <v>219</v>
       </c>
-      <c r="I39" t="s">
+      <c r="K39" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>1984</v>
       </c>
       <c r="B40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C40">
@@ -2982,26 +3286,34 @@
         <v>1.2181828954795768</v>
       </c>
       <c r="F40">
+        <f>'labour '!B47/'labour '!$B$36</f>
+        <v>1.1627715002116374</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>1.1627715002116374</v>
+      </c>
+      <c r="H40">
         <f>'Energy data'!K27/'Energy data'!$K$16</f>
         <v>1.2652217003490329</v>
       </c>
-      <c r="G40">
+      <c r="I40">
         <f>'Energy data'!R27/'Energy data'!$R$16</f>
         <v>1.2445989103888784</v>
       </c>
-      <c r="H40" t="s">
+      <c r="J40" t="s">
         <v>219</v>
       </c>
-      <c r="I40" t="s">
+      <c r="K40" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>1985</v>
       </c>
       <c r="B41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C41">
@@ -3017,26 +3329,34 @@
         <v>1.2225080027933586</v>
       </c>
       <c r="F41">
+        <f>'labour '!B48/'labour '!$B$36</f>
+        <v>1.1581279285886608</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>1.1581279285886608</v>
+      </c>
+      <c r="H41">
         <f>'Energy data'!K28/'Energy data'!$K$16</f>
         <v>1.2770284827853666</v>
       </c>
-      <c r="G41">
+      <c r="I41">
         <f>'Energy data'!R28/'Energy data'!$R$16</f>
         <v>1.2554950216043583</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>219</v>
       </c>
-      <c r="I41" t="s">
+      <c r="K41" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>1986</v>
       </c>
       <c r="B42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C42">
@@ -3052,26 +3372,34 @@
         <v>1.2397767135468609</v>
       </c>
       <c r="F42">
+        <f>'labour '!B49/'labour '!$B$36</f>
+        <v>1.166588114148096</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>1.166588114148096</v>
+      </c>
+      <c r="H42">
         <f>'Energy data'!K29/'Energy data'!$K$16</f>
         <v>1.2796570000430907</v>
       </c>
-      <c r="G42">
+      <c r="I42">
         <f>'Energy data'!R29/'Energy data'!$R$16</f>
         <v>1.2483561901183542</v>
       </c>
-      <c r="H42" t="s">
+      <c r="J42" t="s">
         <v>219</v>
       </c>
-      <c r="I42" t="s">
+      <c r="K42" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>1987</v>
       </c>
       <c r="B43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C43">
@@ -3087,26 +3415,34 @@
         <v>1.2591894677176954</v>
       </c>
       <c r="F43">
+        <f>'labour '!B50/'labour '!$B$36</f>
+        <v>1.1775524204540055</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>1.1775524204540055</v>
+      </c>
+      <c r="H43">
         <f>'Energy data'!K30/'Energy data'!$K$16</f>
         <v>1.3440341276339038</v>
       </c>
-      <c r="G43">
+      <c r="I43">
         <f>'Energy data'!R30/'Energy data'!$R$16</f>
         <v>1.2854906381113407</v>
       </c>
-      <c r="H43" t="s">
+      <c r="J43" t="s">
         <v>219</v>
       </c>
-      <c r="I43" t="s">
+      <c r="K43" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>1988</v>
       </c>
       <c r="B44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C44">
@@ -3122,26 +3458,34 @@
         <v>1.2818596722486471</v>
       </c>
       <c r="F44">
+        <f>'labour '!B51/'labour '!$B$36</f>
+        <v>1.191707536862461</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>1.191707536862461</v>
+      </c>
+      <c r="H44">
         <f>'Energy data'!K31/'Energy data'!$K$16</f>
         <v>1.3825569871159566</v>
       </c>
-      <c r="G44">
+      <c r="I44">
         <f>'Energy data'!R31/'Energy data'!$R$16</f>
         <v>1.3523702172960108</v>
       </c>
-      <c r="H44" t="s">
+      <c r="J44" t="s">
         <v>219</v>
       </c>
-      <c r="I44" t="s">
+      <c r="K44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>1989</v>
       </c>
       <c r="B45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C45">
@@ -3157,26 +3501,34 @@
         <v>1.2992227845397488</v>
       </c>
       <c r="F45">
+        <f>'labour '!B52/'labour '!$B$36</f>
+        <v>1.1991033083406899</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>1.1991033083406899</v>
+      </c>
+      <c r="H45">
         <f>'Energy data'!K32/'Energy data'!$K$16</f>
         <v>1.4230620071530142</v>
       </c>
-      <c r="G45">
+      <c r="I45">
         <f>'Energy data'!R32/'Energy data'!$R$16</f>
         <v>1.3832425324065374</v>
       </c>
-      <c r="H45" t="s">
+      <c r="J45" t="s">
         <v>219</v>
       </c>
-      <c r="I45" t="s">
+      <c r="K45" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>1990</v>
       </c>
       <c r="B46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C46">
@@ -3192,26 +3544,34 @@
         <v>1.3080902446782243</v>
       </c>
       <c r="F46">
+        <f>'labour '!B53/'labour '!$B$36</f>
+        <v>1.1955063273323741</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>1.1955063273323741</v>
+      </c>
+      <c r="H46">
         <f>'Energy data'!K33/'Energy data'!$K$16</f>
         <v>1.4841211703365365</v>
       </c>
-      <c r="G46">
+      <c r="I46">
         <f>'Energy data'!R33/'Energy data'!$R$16</f>
         <v>1.3929488383743502</v>
       </c>
-      <c r="H46" t="s">
+      <c r="J46" t="s">
         <v>219</v>
       </c>
-      <c r="I46" t="s">
+      <c r="K46" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>1991</v>
       </c>
       <c r="B47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C47">
@@ -3227,26 +3587,34 @@
         <v>1.3054791434282975</v>
       </c>
       <c r="F47">
+        <f>'labour '!B54/'labour '!$B$36</f>
+        <v>1.1786460081415622</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>1.1786460081415622</v>
+      </c>
+      <c r="H47">
         <f>'Energy data'!K34/'Energy data'!$K$16</f>
         <v>1.4777868746498903</v>
       </c>
-      <c r="G47">
+      <c r="I47">
         <f>'Energy data'!R34/'Energy data'!$R$16</f>
         <v>1.3740998183981465</v>
       </c>
-      <c r="H47" t="s">
+      <c r="J47" t="s">
         <v>219</v>
       </c>
-      <c r="I47" t="s">
+      <c r="K47" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>1992</v>
       </c>
       <c r="B48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C48">
@@ -3262,26 +3630,34 @@
         <v>1.3045697437852499</v>
       </c>
       <c r="F48">
+        <f>'labour '!B55/'labour '!$B$36</f>
+        <v>1.162983015105215</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>1.162983015105215</v>
+      </c>
+      <c r="H48">
         <f>'Energy data'!K35/'Energy data'!$K$16</f>
         <v>1.4669280820442108</v>
       </c>
-      <c r="G48">
+      <c r="I48">
         <f>'Energy data'!R35/'Energy data'!$R$16</f>
         <v>1.332957605360386</v>
       </c>
-      <c r="H48" t="s">
+      <c r="J48" t="s">
         <v>219</v>
       </c>
-      <c r="I48" t="s">
+      <c r="K48" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>1993</v>
       </c>
       <c r="B49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C49">
@@ -3297,26 +3673,34 @@
         <v>1.3071701709914374</v>
       </c>
       <c r="F49">
+        <f>'labour '!B56/'labour '!$B$36</f>
+        <v>1.1493052921992661</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>1.1493052921992661</v>
+      </c>
+      <c r="H49">
         <f>'Energy data'!K36/'Energy data'!$K$16</f>
         <v>1.5544447795923646</v>
       </c>
-      <c r="G49">
+      <c r="I49">
         <f>'Energy data'!R36/'Energy data'!$R$16</f>
         <v>1.3320809067568415</v>
       </c>
-      <c r="H49" t="s">
+      <c r="J49" t="s">
         <v>219</v>
       </c>
-      <c r="I49" t="s">
+      <c r="K49" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>1994</v>
       </c>
       <c r="B50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C50">
@@ -3332,26 +3716,34 @@
         <v>1.3141509044561606</v>
       </c>
       <c r="F50">
+        <f>'labour '!B57/'labour '!$B$36</f>
+        <v>1.1446165767907364</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>1.1446165767907364</v>
+      </c>
+      <c r="H50">
         <f>'Energy data'!K37/'Energy data'!$K$16</f>
         <v>1.6020597233593314</v>
       </c>
-      <c r="G50">
+      <c r="I50">
         <f>'Energy data'!R37/'Energy data'!$R$16</f>
         <v>1.3687143841192309</v>
       </c>
-      <c r="H50" t="s">
+      <c r="J50" t="s">
         <v>219</v>
       </c>
-      <c r="I50" t="s">
+      <c r="K50" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>1995</v>
       </c>
       <c r="B51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C51">
@@ -3367,26 +3759,34 @@
         <v>1.3290565756177866</v>
       </c>
       <c r="F51">
+        <f>'labour '!B58/'labour '!$B$36</f>
+        <v>1.1458454489284469</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>1.1458454489284469</v>
+      </c>
+      <c r="H51">
         <f>'Energy data'!K38/'Energy data'!$K$16</f>
         <v>1.7083638557331844</v>
       </c>
-      <c r="G51">
+      <c r="I51">
         <f>'Energy data'!R38/'Energy data'!$R$16</f>
         <v>1.4638361826037947</v>
       </c>
-      <c r="H51" t="s">
+      <c r="J51" t="s">
         <v>219</v>
       </c>
-      <c r="I51" t="s">
+      <c r="K51" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>1996</v>
       </c>
       <c r="B52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C52">
@@ -3402,26 +3802,34 @@
         <v>1.3478509939555294</v>
       </c>
       <c r="F52">
+        <f>'labour '!B59/'labour '!$B$36</f>
+        <v>1.1560121643684795</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>1.1560121643684795</v>
+      </c>
+      <c r="H52">
         <f>'Energy data'!K39/'Energy data'!$K$16</f>
         <v>1.7874779161459904</v>
       </c>
-      <c r="G52">
+      <c r="I52">
         <f>'Energy data'!R39/'Energy data'!$R$16</f>
         <v>1.5423633289498402</v>
       </c>
-      <c r="H52" t="s">
+      <c r="J52" t="s">
         <v>219</v>
       </c>
-      <c r="I52" t="s">
+      <c r="K52" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>1997</v>
       </c>
       <c r="B53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C53">
@@ -3437,26 +3845,34 @@
         <v>1.3516425773294416</v>
       </c>
       <c r="F53">
+        <f>'labour '!B60/'labour '!$B$36</f>
+        <v>1.1528869079700799</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>1.1528869079700799</v>
+      </c>
+      <c r="H53">
         <f>'Energy data'!K40/'Energy data'!$K$16</f>
         <v>1.9469987503770414</v>
       </c>
-      <c r="G53">
+      <c r="I53">
         <f>'Energy data'!R40/'Energy data'!$R$16</f>
         <v>1.6019788339908574</v>
       </c>
-      <c r="H53" t="s">
+      <c r="J53" t="s">
         <v>219</v>
       </c>
-      <c r="I53" t="s">
+      <c r="K53" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>1998</v>
       </c>
       <c r="B54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="C54">
@@ -3472,26 +3888,34 @@
         <v>1.3374286861121705</v>
       </c>
       <c r="F54">
+        <f>'labour '!B61/'labour '!$B$36</f>
+        <v>1.1355485379690513</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>1.1355485379690513</v>
+      </c>
+      <c r="H54">
         <f>'Energy data'!K41/'Energy data'!$K$16</f>
         <v>1.8943422243288659</v>
       </c>
-      <c r="G54">
+      <c r="I54">
         <f>'Energy data'!R41/'Energy data'!$R$16</f>
         <v>1.5893293255682888</v>
       </c>
-      <c r="H54" t="s">
+      <c r="J54" t="s">
         <v>219</v>
       </c>
-      <c r="I54" t="s">
+      <c r="K54" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>1999</v>
       </c>
       <c r="B55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C55">
@@ -3507,26 +3931,34 @@
         <v>1.3341025545279603</v>
       </c>
       <c r="F55">
+        <f>'labour '!B62/'labour '!$B$36</f>
+        <v>1.1294418119467229</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>1.1294418119467229</v>
+      </c>
+      <c r="H55">
         <f>'Energy data'!K42/'Energy data'!$K$16</f>
         <v>1.8629292885767232</v>
       </c>
-      <c r="G55">
+      <c r="I55">
         <f>'Energy data'!R42/'Energy data'!$R$16</f>
         <v>1.5453065314045964</v>
       </c>
-      <c r="H55" t="s">
+      <c r="J55" t="s">
         <v>219</v>
       </c>
-      <c r="I55" t="s">
+      <c r="K55" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>2000</v>
       </c>
       <c r="B56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="C56">
@@ -3542,26 +3974,34 @@
         <v>1.320319309319465</v>
       </c>
       <c r="F56">
+        <f>'labour '!B63/'labour '!$B$36</f>
+        <v>1.1206713526740804</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>1.1206713526740804</v>
+      </c>
+      <c r="H56">
         <f>'Energy data'!K43/'Energy data'!$K$16</f>
         <v>1.9042961175507396</v>
       </c>
-      <c r="G56">
+      <c r="I56">
         <f>'Energy data'!R43/'Energy data'!$R$16</f>
         <v>1.5663472978896613</v>
       </c>
-      <c r="H56" t="s">
+      <c r="J56" t="s">
         <v>219</v>
       </c>
-      <c r="I56" t="s">
+      <c r="K56" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>2001</v>
       </c>
       <c r="B57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="C57">
@@ -3577,26 +4017,34 @@
         <v>1.2687051452501636</v>
       </c>
       <c r="F57">
+        <f>'labour '!B64/'labour '!$B$36</f>
+        <v>1.1096287388075015</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>1.1096287388075015</v>
+      </c>
+      <c r="H57">
         <f>'Energy data'!K44/'Energy data'!$K$16</f>
         <v>1.8556470030594225</v>
       </c>
-      <c r="G57">
+      <c r="I57">
         <f>'Energy data'!R44/'Energy data'!$R$16</f>
         <v>1.5470599286116851</v>
       </c>
-      <c r="H57" t="s">
+      <c r="J57" t="s">
         <v>219</v>
       </c>
-      <c r="I57" t="s">
+      <c r="K57" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:11">
       <c r="A58">
         <v>2002</v>
       </c>
       <c r="B58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="C58">
@@ -3612,26 +4060,34 @@
         <v>1.2565404162051708</v>
       </c>
       <c r="F58">
+        <f>'labour '!B65/'labour '!$B$36</f>
+        <v>1.1549048899999546</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>1.1549048899999546</v>
+      </c>
+      <c r="H58">
         <f>'Energy data'!K45/'Energy data'!$K$16</f>
         <v>1.952859051148361</v>
       </c>
-      <c r="G58">
+      <c r="I58">
         <f>'Energy data'!R45/'Energy data'!$R$16</f>
         <v>1.6297200826601539</v>
       </c>
-      <c r="H58" t="s">
+      <c r="J58" t="s">
         <v>219</v>
       </c>
-      <c r="I58" t="s">
+      <c r="K58" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:11">
       <c r="A59">
         <v>2003</v>
       </c>
       <c r="B59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="C59">
@@ -3647,26 +4103,34 @@
         <v>1.2841687463472171</v>
       </c>
       <c r="F59">
+        <f>'labour '!B66/'labour '!$B$36</f>
+        <v>1.1445141682138202</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>1.1445141682138202</v>
+      </c>
+      <c r="H59">
         <f>'Energy data'!K46/'Energy data'!$K$16</f>
         <v>1.9979747489981472</v>
       </c>
-      <c r="G59">
+      <c r="I59">
         <f>'Energy data'!R46/'Energy data'!$R$16</f>
         <v>1.6952846139395077</v>
       </c>
-      <c r="H59" t="s">
+      <c r="J59" t="s">
         <v>219</v>
       </c>
-      <c r="I59" t="s">
+      <c r="K59" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:11">
       <c r="A60">
         <v>2004</v>
       </c>
       <c r="B60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="C60">
@@ -3682,26 +4146,34 @@
         <v>1.3178330948213797</v>
       </c>
       <c r="F60">
+        <f>'labour '!B67/'labour '!$B$36</f>
+        <v>1.152710785725148</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>1.152710785725148</v>
+      </c>
+      <c r="H60">
         <f>'Energy data'!K47/'Energy data'!$K$16</f>
         <v>2.0863101650364113</v>
       </c>
-      <c r="G60">
+      <c r="I60">
         <f>'Energy data'!R47/'Energy data'!$R$16</f>
         <v>1.7300394514371593</v>
       </c>
-      <c r="H60" t="s">
+      <c r="J60" t="s">
         <v>219</v>
       </c>
-      <c r="I60" t="s">
+      <c r="K60" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:11">
       <c r="A61">
         <v>2005</v>
       </c>
       <c r="B61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="C61">
@@ -3717,26 +4189,34 @@
         <v>1.3502139920474661</v>
       </c>
       <c r="F61">
+        <f>'labour '!B68/'labour '!$B$36</f>
+        <v>1.1489795614486409</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>1.1489795614486409</v>
+      </c>
+      <c r="H61">
         <f>'Energy data'!K48/'Energy data'!$K$16</f>
         <v>2.1118197095703879</v>
       </c>
-      <c r="G61">
+      <c r="I61">
         <f>'Energy data'!R48/'Energy data'!$R$16</f>
         <v>1.7472603168639236</v>
       </c>
-      <c r="H61" t="s">
+      <c r="J61" t="s">
         <v>219</v>
       </c>
-      <c r="I61" t="s">
+      <c r="K61" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:11">
       <c r="A62">
         <v>2006</v>
       </c>
       <c r="B62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="C62">
@@ -3752,26 +4232,34 @@
         <v>1.40852213995732</v>
       </c>
       <c r="F62">
+        <f>'labour '!B69/'labour '!$B$36</f>
+        <v>1.1955812540833528</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>1.1955812540833528</v>
+      </c>
+      <c r="H62">
         <f>'Energy data'!K49/'Energy data'!$K$16</f>
         <v>2.0354634377558498</v>
       </c>
-      <c r="G62">
+      <c r="I62">
         <f>'Energy data'!R49/'Energy data'!$R$16</f>
         <v>1.7419375039138327</v>
       </c>
-      <c r="H62" t="s">
+      <c r="J62" t="s">
         <v>219</v>
       </c>
-      <c r="I62" t="s">
+      <c r="K62" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:11">
       <c r="A63">
         <v>2007</v>
       </c>
       <c r="B63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="C63">
@@ -3787,26 +4275,34 @@
         <v>1.4508534102143162</v>
       </c>
       <c r="F63">
+        <f>'labour '!B70/'labour '!$B$36</f>
+        <v>1.212780495787539</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>1.212780495787539</v>
+      </c>
+      <c r="H63">
         <f>'Energy data'!K50/'Energy data'!$K$16</f>
         <v>2.1911923126642825</v>
       </c>
-      <c r="G63">
+      <c r="I63">
         <f>'Energy data'!R50/'Energy data'!$R$16</f>
         <v>1.9090112092178595</v>
       </c>
-      <c r="H63" t="s">
+      <c r="J63" t="s">
         <v>219</v>
       </c>
-      <c r="I63" t="s">
+      <c r="K63" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:11">
       <c r="A64">
         <v>2008</v>
       </c>
       <c r="B64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="C64">
@@ -3822,26 +4318,34 @@
         <v>1.5325774782263533</v>
       </c>
       <c r="F64">
+        <f>'labour '!B71/'labour '!$B$36</f>
+        <v>1.2059356699631989</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>1.2059356699631989</v>
+      </c>
+      <c r="H64">
         <f>'Energy data'!K51/'Energy data'!$K$16</f>
         <v>2.3412332485887881</v>
       </c>
-      <c r="G64">
+      <c r="I64">
         <f>'Energy data'!R51/'Energy data'!$R$16</f>
         <v>1.8536539545369148</v>
       </c>
-      <c r="H64" t="s">
+      <c r="J64" t="s">
         <v>219</v>
       </c>
-      <c r="I64" t="s">
+      <c r="K64" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:11">
       <c r="A65">
         <v>2009</v>
       </c>
       <c r="B65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="C65">
@@ -3857,26 +4361,34 @@
         <v>1.4913642319808285</v>
       </c>
       <c r="F65">
+        <f>'labour '!B72/'labour '!$B$36</f>
+        <v>1.1642851762823798</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>1.1642851762823798</v>
+      </c>
+      <c r="H65">
         <f>'Energy data'!K52/'Energy data'!$K$16</f>
         <v>2.21209117938553</v>
       </c>
-      <c r="G65">
+      <c r="I65">
         <f>'Energy data'!R52/'Energy data'!$R$16</f>
         <v>1.8879704427327944</v>
       </c>
-      <c r="H65" t="s">
+      <c r="J65" t="s">
         <v>219</v>
       </c>
-      <c r="I65" t="s">
+      <c r="K65" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:11">
       <c r="A66">
         <v>2010</v>
       </c>
       <c r="B66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C66">
@@ -3892,26 +4404,34 @@
         <v>1.4489218182400709</v>
       </c>
       <c r="F66">
+        <f>'labour '!B73/'labour '!$B$36</f>
+        <v>1.1457617583390758</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>1.1457617583390758</v>
+      </c>
+      <c r="H66">
         <f>'Energy data'!K53/'Energy data'!$K$16</f>
         <v>2.2680225793941484</v>
       </c>
-      <c r="G66">
+      <c r="I66">
         <f>'Energy data'!R53/'Energy data'!$R$16</f>
         <v>1.8787651073955787</v>
       </c>
-      <c r="H66" t="s">
+      <c r="J66" t="s">
         <v>219</v>
       </c>
-      <c r="I66" t="s">
+      <c r="K66" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:11">
       <c r="A67">
         <v>2011</v>
       </c>
       <c r="B67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="C67">
@@ -3927,26 +4447,34 @@
         <v>1.4785314877267177</v>
       </c>
       <c r="F67">
+        <f>'labour '!B74/'labour '!$B$36</f>
+        <v>1.1603708644982589</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G69" si="3">F67</f>
+        <v>1.1603708644982589</v>
+      </c>
+      <c r="H67">
         <f>'Energy data'!K54/'Energy data'!$K$16</f>
         <v>2.2600077562804324</v>
       </c>
-      <c r="G67">
+      <c r="I67">
         <f>'Energy data'!R54/'Energy data'!$R$16</f>
         <v>1.9590456509487129</v>
       </c>
-      <c r="H67" t="s">
+      <c r="J67" t="s">
         <v>219</v>
       </c>
-      <c r="I67" t="s">
+      <c r="K67" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:11">
       <c r="A68">
         <v>2012</v>
       </c>
       <c r="B68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="C68">
@@ -3961,25 +4489,33 @@
         <f>'labour '!C75/'labour '!$C$36</f>
         <v>1.5159882381675731</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68">
+        <f>'labour '!B75/'labour '!$B$36</f>
+        <v>1.1798335520788421</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="3"/>
+        <v>1.1798335520788421</v>
+      </c>
+      <c r="H68" t="s">
         <v>216</v>
       </c>
-      <c r="G68" t="s">
+      <c r="I68" t="s">
         <v>216</v>
       </c>
-      <c r="H68" t="s">
+      <c r="J68" t="s">
         <v>219</v>
       </c>
-      <c r="I68" t="s">
+      <c r="K68" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:11">
       <c r="A69">
         <v>2013</v>
       </c>
       <c r="B69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="C69">
@@ -3994,16 +4530,24 @@
         <f>'labour '!C76/'labour '!$C$36</f>
         <v>1.5623691249968692</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69">
+        <f>'labour '!B76/'labour '!$B$36</f>
+        <v>1.1894539153510799</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="3"/>
+        <v>1.1894539153510799</v>
+      </c>
+      <c r="H69" t="s">
         <v>216</v>
       </c>
-      <c r="G69" t="s">
+      <c r="I69" t="s">
         <v>216</v>
       </c>
-      <c r="H69" t="s">
+      <c r="J69" t="s">
         <v>219</v>
       </c>
-      <c r="I69" t="s">
+      <c r="K69" t="s">
         <v>218</v>
       </c>
     </row>
@@ -11099,7 +11643,7 @@
   <dimension ref="A8:AD76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
@@ -15413,10 +15957,10 @@
   <dimension ref="A1:AT56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L54" sqref="L54"/>
+      <selection pane="bottomRight" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updates to SUN data.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/SUN/SUN Data.xlsx
+++ b/data/Excel Workbooks/SUN/SUN Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="25040" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28160" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Indexed" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="222">
   <si>
     <t>Year</t>
   </si>
@@ -667,9 +667,6 @@
   </si>
   <si>
     <t>iK</t>
-  </si>
-  <si>
-    <t>iL</t>
   </si>
   <si>
     <t>iQp</t>
@@ -1690,20 +1687,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G69"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
         <v>211</v>
@@ -1712,10 +1709,10 @@
         <v>212</v>
       </c>
       <c r="E1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" t="s">
         <v>221</v>
-      </c>
-      <c r="F1" t="s">
-        <v>222</v>
       </c>
       <c r="G1" t="s">
         <v>213</v>
@@ -1724,16 +1721,13 @@
         <v>214</v>
       </c>
       <c r="I1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J1" t="s">
-        <v>217</v>
-      </c>
-      <c r="K1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1946</v>
       </c>
@@ -1750,29 +1744,25 @@
         <v>0.22679934864156337</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G2" t="str">
-        <f>F2</f>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G2" t="s">
+        <v>215</v>
       </c>
       <c r="H2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J2" t="s">
-        <v>219</v>
-      </c>
-      <c r="K2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1947</v>
       </c>
@@ -1789,29 +1779,25 @@
         <v>0.24260125204275501</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G66" si="1">F3</f>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G3" t="s">
+        <v>215</v>
       </c>
       <c r="H3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J3" t="s">
-        <v>219</v>
-      </c>
-      <c r="K3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1948</v>
       </c>
@@ -1828,29 +1814,25 @@
         <v>0.26422995305021169</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G4" t="s">
+        <v>215</v>
       </c>
       <c r="H4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J4" t="s">
-        <v>219</v>
-      </c>
-      <c r="K4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1949</v>
       </c>
@@ -1867,29 +1849,25 @@
         <v>0.28587680381348152</v>
       </c>
       <c r="E5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G5" t="s">
+        <v>215</v>
       </c>
       <c r="H5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J5" t="s">
-        <v>219</v>
-      </c>
-      <c r="K5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>1950</v>
       </c>
@@ -1906,29 +1884,25 @@
         <v>0.3033310609839055</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>216</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G6" t="s">
+        <v>215</v>
       </c>
       <c r="H6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I6" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J6" t="s">
-        <v>219</v>
-      </c>
-      <c r="K6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>1951</v>
       </c>
@@ -1945,29 +1919,25 @@
         <v>0.31902188787952046</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F7" t="s">
-        <v>216</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G7" t="s">
+        <v>215</v>
       </c>
       <c r="H7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J7" t="s">
-        <v>219</v>
-      </c>
-      <c r="K7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>1952</v>
       </c>
@@ -1984,29 +1954,25 @@
         <v>0.33768782274803277</v>
       </c>
       <c r="E8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G8" t="s">
+        <v>215</v>
       </c>
       <c r="H8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I8" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J8" t="s">
-        <v>219</v>
-      </c>
-      <c r="K8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>1953</v>
       </c>
@@ -2023,29 +1989,25 @@
         <v>0.36016593232754646</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F9" t="s">
-        <v>216</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G9" t="s">
+        <v>215</v>
       </c>
       <c r="H9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I9" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J9" t="s">
-        <v>219</v>
-      </c>
-      <c r="K9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1954</v>
       </c>
@@ -2062,29 +2024,25 @@
         <v>0.38246254434892835</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G10" t="s">
+        <v>215</v>
       </c>
       <c r="H10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I10" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J10" t="s">
-        <v>219</v>
-      </c>
-      <c r="K10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>1955</v>
       </c>
@@ -2101,29 +2059,25 @@
         <v>0.40271984980714071</v>
       </c>
       <c r="E11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G11" t="s">
+        <v>215</v>
       </c>
       <c r="H11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J11" t="s">
-        <v>219</v>
-      </c>
-      <c r="K11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>1956</v>
       </c>
@@ -2140,29 +2094,25 @@
         <v>0.42096253237008951</v>
       </c>
       <c r="E12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F12" t="s">
-        <v>216</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G12" t="s">
+        <v>215</v>
       </c>
       <c r="H12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I12" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>1957</v>
       </c>
@@ -2179,29 +2129,25 @@
         <v>0.4405904042967006</v>
       </c>
       <c r="E13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
-        <v>216</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G13" t="s">
+        <v>215</v>
       </c>
       <c r="H13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I13" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J13" t="s">
-        <v>219</v>
-      </c>
-      <c r="K13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>1958</v>
       </c>
@@ -2218,29 +2164,25 @@
         <v>0.46439562402127443</v>
       </c>
       <c r="E14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G14" t="s">
+        <v>215</v>
       </c>
       <c r="H14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I14" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J14" t="s">
-        <v>219</v>
-      </c>
-      <c r="K14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>1959</v>
       </c>
@@ -2257,29 +2199,25 @@
         <v>0.48492444982645205</v>
       </c>
       <c r="E15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F15" t="s">
-        <v>216</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G15" t="s">
+        <v>215</v>
       </c>
       <c r="H15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I15" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J15" t="s">
-        <v>219</v>
-      </c>
-      <c r="K15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>1960</v>
       </c>
@@ -2296,29 +2234,25 @@
         <v>0.50562751328743627</v>
       </c>
       <c r="E16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F16" t="s">
-        <v>216</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G16" t="s">
+        <v>215</v>
       </c>
       <c r="H16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I16" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J16" t="s">
-        <v>219</v>
-      </c>
-      <c r="K16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>1961</v>
       </c>
@@ -2335,29 +2269,25 @@
         <v>0.52389124956712829</v>
       </c>
       <c r="E17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F17" t="s">
-        <v>216</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G17" t="s">
+        <v>215</v>
       </c>
       <c r="H17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J17" t="s">
-        <v>219</v>
-      </c>
-      <c r="K17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>1962</v>
       </c>
@@ -2374,29 +2304,25 @@
         <v>0.54041260928875468</v>
       </c>
       <c r="E18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F18" t="s">
-        <v>216</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G18" t="s">
+        <v>215</v>
       </c>
       <c r="H18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I18" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J18" t="s">
-        <v>219</v>
-      </c>
-      <c r="K18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>1963</v>
       </c>
@@ -2413,29 +2339,25 @@
         <v>0.56220393210829744</v>
       </c>
       <c r="E19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F19" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G19" t="s">
+        <v>215</v>
       </c>
       <c r="H19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J19" t="s">
-        <v>219</v>
-      </c>
-      <c r="K19" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>1964</v>
       </c>
@@ -2452,29 +2374,25 @@
         <v>0.5914054372312475</v>
       </c>
       <c r="E20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F20" t="s">
-        <v>216</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G20" t="s">
+        <v>215</v>
       </c>
       <c r="H20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I20" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J20" t="s">
-        <v>219</v>
-      </c>
-      <c r="K20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>1965</v>
       </c>
@@ -2491,29 +2409,25 @@
         <v>0.62842658314875033</v>
       </c>
       <c r="E21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
-        <v>216</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G21" t="s">
+        <v>215</v>
       </c>
       <c r="H21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I21" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J21" t="s">
-        <v>219</v>
-      </c>
-      <c r="K21" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>1966</v>
       </c>
@@ -2530,29 +2444,25 @@
         <v>0.66330315391936712</v>
       </c>
       <c r="E22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F22" t="s">
-        <v>216</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G22" t="s">
+        <v>215</v>
       </c>
       <c r="H22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I22" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J22" t="s">
-        <v>219</v>
-      </c>
-      <c r="K22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>1967</v>
       </c>
@@ -2569,29 +2479,25 @@
         <v>0.69764612186907637</v>
       </c>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F23" t="s">
-        <v>216</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G23" t="s">
+        <v>215</v>
       </c>
       <c r="H23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I23" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J23" t="s">
-        <v>219</v>
-      </c>
-      <c r="K23" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>1968</v>
       </c>
@@ -2608,29 +2514,25 @@
         <v>0.73256480007317981</v>
       </c>
       <c r="E24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F24" t="s">
-        <v>216</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G24" t="s">
+        <v>215</v>
       </c>
       <c r="H24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I24" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J24" t="s">
-        <v>219</v>
-      </c>
-      <c r="K24" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>1969</v>
       </c>
@@ -2647,29 +2549,25 @@
         <v>0.77404062205747082</v>
       </c>
       <c r="E25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F25" t="s">
-        <v>216</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+        <v>215</v>
+      </c>
+      <c r="G25" t="s">
+        <v>215</v>
       </c>
       <c r="H25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J25" t="s">
-        <v>219</v>
-      </c>
-      <c r="K25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>1970</v>
       </c>
@@ -2693,24 +2591,20 @@
         <f>'labour '!B33/'labour '!$B$36</f>
         <v>0.92333577712232928</v>
       </c>
-      <c r="G26">
-        <f t="shared" si="1"/>
-        <v>0.92333577712232928</v>
+      <c r="G26" t="s">
+        <v>215</v>
       </c>
       <c r="H26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I26" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J26" t="s">
-        <v>219</v>
-      </c>
-      <c r="K26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>1971</v>
       </c>
@@ -2734,24 +2628,20 @@
         <f>'labour '!B34/'labour '!$B$36</f>
         <v>0.9445901877653603</v>
       </c>
-      <c r="G27">
-        <f t="shared" si="1"/>
-        <v>0.9445901877653603</v>
+      <c r="G27" t="s">
+        <v>215</v>
       </c>
       <c r="H27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I27" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J27" t="s">
-        <v>219</v>
-      </c>
-      <c r="K27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>1972</v>
       </c>
@@ -2775,24 +2665,20 @@
         <f>'labour '!B35/'labour '!$B$36</f>
         <v>0.96118443852064028</v>
       </c>
-      <c r="G28">
-        <f t="shared" si="1"/>
-        <v>0.96118443852064028</v>
+      <c r="G28" t="s">
+        <v>215</v>
       </c>
       <c r="H28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I28" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J28" t="s">
-        <v>219</v>
-      </c>
-      <c r="K28" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>1973</v>
       </c>
@@ -2817,30 +2703,26 @@
         <v>1</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H29">
         <f>'Energy data'!K16/'Energy data'!$K$16</f>
         <v>1</v>
       </c>
-      <c r="I29">
+      <c r="H29">
         <f>'Energy data'!R16/'Energy data'!$R$16</f>
         <v>1</v>
       </c>
+      <c r="I29" t="s">
+        <v>218</v>
+      </c>
       <c r="J29" t="s">
-        <v>219</v>
-      </c>
-      <c r="K29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>1974</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:B69" si="2">A30-$A$29</f>
+        <f t="shared" ref="B30:B69" si="1">A30-$A$29</f>
         <v>1</v>
       </c>
       <c r="C30">
@@ -2860,30 +2742,26 @@
         <v>1.0358570789501769</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
-        <v>1.0358570789501769</v>
-      </c>
-      <c r="H30">
         <f>'Energy data'!K17/'Energy data'!$K$16</f>
         <v>1.029990951006162</v>
       </c>
-      <c r="I30">
+      <c r="H30">
         <f>'Energy data'!R17/'Energy data'!$R$16</f>
         <v>1.0051975702924416</v>
       </c>
+      <c r="I30" t="s">
+        <v>218</v>
+      </c>
       <c r="J30" t="s">
-        <v>219</v>
-      </c>
-      <c r="K30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>1975</v>
       </c>
       <c r="B31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C31">
@@ -2903,30 +2781,26 @@
         <v>1.0680120517764264</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
-        <v>1.0680120517764264</v>
-      </c>
-      <c r="H31">
         <f>'Energy data'!K18/'Energy data'!$K$16</f>
         <v>1.1190589046408412</v>
       </c>
-      <c r="I31">
+      <c r="H31">
         <f>'Energy data'!R18/'Energy data'!$R$16</f>
         <v>1.0780261757154486</v>
       </c>
+      <c r="I31" t="s">
+        <v>218</v>
+      </c>
       <c r="J31" t="s">
-        <v>219</v>
-      </c>
-      <c r="K31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>1976</v>
       </c>
       <c r="B32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C32">
@@ -2946,30 +2820,26 @@
         <v>1.0768993110404073</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
-        <v>1.0768993110404073</v>
-      </c>
-      <c r="H32">
         <f>'Energy data'!K19/'Energy data'!$K$16</f>
         <v>1.168009652260094</v>
       </c>
-      <c r="I32">
+      <c r="H32">
         <f>'Energy data'!R19/'Energy data'!$R$16</f>
         <v>1.1149101383931368</v>
       </c>
+      <c r="I32" t="s">
+        <v>218</v>
+      </c>
       <c r="J32" t="s">
-        <v>219</v>
-      </c>
-      <c r="K32" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>1977</v>
       </c>
       <c r="B33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C33">
@@ -2989,30 +2859,26 @@
         <v>1.0623062619489441</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
-        <v>1.0623062619489441</v>
-      </c>
-      <c r="H33">
         <f>'Energy data'!K20/'Energy data'!$K$16</f>
         <v>1.1740423148188048</v>
       </c>
-      <c r="I33">
+      <c r="H33">
         <f>'Energy data'!R20/'Energy data'!$R$16</f>
         <v>1.089172772246227</v>
       </c>
+      <c r="I33" t="s">
+        <v>218</v>
+      </c>
       <c r="J33" t="s">
-        <v>219</v>
-      </c>
-      <c r="K33" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>1978</v>
       </c>
       <c r="B34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C34">
@@ -3032,30 +2898,26 @@
         <v>1.0643549715500999</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
-        <v>1.0643549715500999</v>
-      </c>
-      <c r="H34">
         <f>'Energy data'!K21/'Energy data'!$K$16</f>
         <v>1.075537553324428</v>
       </c>
-      <c r="I34">
+      <c r="H34">
         <f>'Energy data'!R21/'Energy data'!$R$16</f>
         <v>1.1509174024672801</v>
       </c>
+      <c r="I34" t="s">
+        <v>218</v>
+      </c>
       <c r="J34" t="s">
-        <v>219</v>
-      </c>
-      <c r="K34" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>1979</v>
       </c>
       <c r="B35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C35">
@@ -3075,30 +2937,26 @@
         <v>1.0791226334849746</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
-        <v>1.0791226334849746</v>
-      </c>
-      <c r="H35">
         <f>'Energy data'!K22/'Energy data'!$K$16</f>
         <v>1.0948851639591504</v>
       </c>
-      <c r="I35">
+      <c r="H35">
         <f>'Energy data'!R22/'Energy data'!$R$16</f>
         <v>1.1403343978959233</v>
       </c>
+      <c r="I35" t="s">
+        <v>218</v>
+      </c>
       <c r="J35" t="s">
-        <v>219</v>
-      </c>
-      <c r="K35" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>1980</v>
       </c>
       <c r="B36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C36">
@@ -3118,30 +2976,26 @@
         <v>1.1151765261466215</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
-        <v>1.1151765261466215</v>
-      </c>
-      <c r="H36">
         <f>'Energy data'!K23/'Energy data'!$K$16</f>
         <v>1.1518076442452707</v>
       </c>
-      <c r="I36">
+      <c r="H36">
         <f>'Energy data'!R23/'Energy data'!$R$16</f>
         <v>1.1834178721272464</v>
       </c>
+      <c r="I36" t="s">
+        <v>218</v>
+      </c>
       <c r="J36" t="s">
-        <v>219</v>
-      </c>
-      <c r="K36" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>1981</v>
       </c>
       <c r="B37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C37">
@@ -3161,30 +3015,26 @@
         <v>1.1481994435684739</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
-        <v>1.1481994435684739</v>
-      </c>
-      <c r="H37">
         <f>'Energy data'!K24/'Energy data'!$K$16</f>
         <v>1.2102382901710691</v>
       </c>
-      <c r="I37">
+      <c r="H37">
         <f>'Energy data'!R24/'Energy data'!$R$16</f>
         <v>1.2435969691276849</v>
       </c>
+      <c r="I37" t="s">
+        <v>218</v>
+      </c>
       <c r="J37" t="s">
-        <v>219</v>
-      </c>
-      <c r="K37" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>1982</v>
       </c>
       <c r="B38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C38">
@@ -3204,30 +3054,26 @@
         <v>1.1610506301282266</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
-        <v>1.1610506301282266</v>
-      </c>
-      <c r="H38">
         <f>'Energy data'!K25/'Energy data'!$K$16</f>
         <v>1.2000689447149568</v>
       </c>
-      <c r="I38">
+      <c r="H38">
         <f>'Energy data'!R25/'Energy data'!$R$16</f>
         <v>1.1981965057298516</v>
       </c>
+      <c r="I38" t="s">
+        <v>218</v>
+      </c>
       <c r="J38" t="s">
-        <v>219</v>
-      </c>
-      <c r="K38" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>1983</v>
       </c>
       <c r="B39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C39">
@@ -3247,30 +3093,26 @@
         <v>1.1527824606649568</v>
       </c>
       <c r="G39">
-        <f t="shared" si="1"/>
-        <v>1.1527824606649568</v>
-      </c>
-      <c r="H39">
         <f>'Energy data'!K26/'Energy data'!$K$16</f>
         <v>1.1808075149739305</v>
       </c>
-      <c r="I39">
+      <c r="H39">
         <f>'Energy data'!R26/'Energy data'!$R$16</f>
         <v>1.1678251612499218</v>
       </c>
+      <c r="I39" t="s">
+        <v>218</v>
+      </c>
       <c r="J39" t="s">
-        <v>219</v>
-      </c>
-      <c r="K39" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>1984</v>
       </c>
       <c r="B40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C40">
@@ -3290,30 +3132,26 @@
         <v>1.1627715002116374</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
-        <v>1.1627715002116374</v>
-      </c>
-      <c r="H40">
         <f>'Energy data'!K27/'Energy data'!$K$16</f>
         <v>1.2652217003490329</v>
       </c>
-      <c r="I40">
+      <c r="H40">
         <f>'Energy data'!R27/'Energy data'!$R$16</f>
         <v>1.2445989103888784</v>
       </c>
+      <c r="I40" t="s">
+        <v>218</v>
+      </c>
       <c r="J40" t="s">
-        <v>219</v>
-      </c>
-      <c r="K40" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>1985</v>
       </c>
       <c r="B41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C41">
@@ -3333,30 +3171,26 @@
         <v>1.1581279285886608</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
-        <v>1.1581279285886608</v>
-      </c>
-      <c r="H41">
         <f>'Energy data'!K28/'Energy data'!$K$16</f>
         <v>1.2770284827853666</v>
       </c>
-      <c r="I41">
+      <c r="H41">
         <f>'Energy data'!R28/'Energy data'!$R$16</f>
         <v>1.2554950216043583</v>
       </c>
+      <c r="I41" t="s">
+        <v>218</v>
+      </c>
       <c r="J41" t="s">
-        <v>219</v>
-      </c>
-      <c r="K41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>1986</v>
       </c>
       <c r="B42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C42">
@@ -3376,30 +3210,26 @@
         <v>1.166588114148096</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
-        <v>1.166588114148096</v>
-      </c>
-      <c r="H42">
         <f>'Energy data'!K29/'Energy data'!$K$16</f>
         <v>1.2796570000430907</v>
       </c>
-      <c r="I42">
+      <c r="H42">
         <f>'Energy data'!R29/'Energy data'!$R$16</f>
         <v>1.2483561901183542</v>
       </c>
+      <c r="I42" t="s">
+        <v>218</v>
+      </c>
       <c r="J42" t="s">
-        <v>219</v>
-      </c>
-      <c r="K42" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>1987</v>
       </c>
       <c r="B43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C43">
@@ -3419,30 +3249,26 @@
         <v>1.1775524204540055</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
-        <v>1.1775524204540055</v>
-      </c>
-      <c r="H43">
         <f>'Energy data'!K30/'Energy data'!$K$16</f>
         <v>1.3440341276339038</v>
       </c>
-      <c r="I43">
+      <c r="H43">
         <f>'Energy data'!R30/'Energy data'!$R$16</f>
         <v>1.2854906381113407</v>
       </c>
+      <c r="I43" t="s">
+        <v>218</v>
+      </c>
       <c r="J43" t="s">
-        <v>219</v>
-      </c>
-      <c r="K43" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>1988</v>
       </c>
       <c r="B44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C44">
@@ -3462,30 +3288,26 @@
         <v>1.191707536862461</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
-        <v>1.191707536862461</v>
-      </c>
-      <c r="H44">
         <f>'Energy data'!K31/'Energy data'!$K$16</f>
         <v>1.3825569871159566</v>
       </c>
-      <c r="I44">
+      <c r="H44">
         <f>'Energy data'!R31/'Energy data'!$R$16</f>
         <v>1.3523702172960108</v>
       </c>
+      <c r="I44" t="s">
+        <v>218</v>
+      </c>
       <c r="J44" t="s">
-        <v>219</v>
-      </c>
-      <c r="K44" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>1989</v>
       </c>
       <c r="B45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C45">
@@ -3505,30 +3327,26 @@
         <v>1.1991033083406899</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
-        <v>1.1991033083406899</v>
-      </c>
-      <c r="H45">
         <f>'Energy data'!K32/'Energy data'!$K$16</f>
         <v>1.4230620071530142</v>
       </c>
-      <c r="I45">
+      <c r="H45">
         <f>'Energy data'!R32/'Energy data'!$R$16</f>
         <v>1.3832425324065374</v>
       </c>
+      <c r="I45" t="s">
+        <v>218</v>
+      </c>
       <c r="J45" t="s">
-        <v>219</v>
-      </c>
-      <c r="K45" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>1990</v>
       </c>
       <c r="B46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C46">
@@ -3548,30 +3366,26 @@
         <v>1.1955063273323741</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
-        <v>1.1955063273323741</v>
-      </c>
-      <c r="H46">
         <f>'Energy data'!K33/'Energy data'!$K$16</f>
         <v>1.4841211703365365</v>
       </c>
-      <c r="I46">
+      <c r="H46">
         <f>'Energy data'!R33/'Energy data'!$R$16</f>
         <v>1.3929488383743502</v>
       </c>
+      <c r="I46" t="s">
+        <v>218</v>
+      </c>
       <c r="J46" t="s">
-        <v>219</v>
-      </c>
-      <c r="K46" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>1991</v>
       </c>
       <c r="B47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C47">
@@ -3591,30 +3405,26 @@
         <v>1.1786460081415622</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
-        <v>1.1786460081415622</v>
-      </c>
-      <c r="H47">
         <f>'Energy data'!K34/'Energy data'!$K$16</f>
         <v>1.4777868746498903</v>
       </c>
-      <c r="I47">
+      <c r="H47">
         <f>'Energy data'!R34/'Energy data'!$R$16</f>
         <v>1.3740998183981465</v>
       </c>
+      <c r="I47" t="s">
+        <v>218</v>
+      </c>
       <c r="J47" t="s">
-        <v>219</v>
-      </c>
-      <c r="K47" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>1992</v>
       </c>
       <c r="B48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C48">
@@ -3634,30 +3444,26 @@
         <v>1.162983015105215</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
-        <v>1.162983015105215</v>
-      </c>
-      <c r="H48">
         <f>'Energy data'!K35/'Energy data'!$K$16</f>
         <v>1.4669280820442108</v>
       </c>
-      <c r="I48">
+      <c r="H48">
         <f>'Energy data'!R35/'Energy data'!$R$16</f>
         <v>1.332957605360386</v>
       </c>
+      <c r="I48" t="s">
+        <v>218</v>
+      </c>
       <c r="J48" t="s">
-        <v>219</v>
-      </c>
-      <c r="K48" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>1993</v>
       </c>
       <c r="B49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C49">
@@ -3677,30 +3483,26 @@
         <v>1.1493052921992661</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
-        <v>1.1493052921992661</v>
-      </c>
-      <c r="H49">
         <f>'Energy data'!K36/'Energy data'!$K$16</f>
         <v>1.5544447795923646</v>
       </c>
-      <c r="I49">
+      <c r="H49">
         <f>'Energy data'!R36/'Energy data'!$R$16</f>
         <v>1.3320809067568415</v>
       </c>
+      <c r="I49" t="s">
+        <v>218</v>
+      </c>
       <c r="J49" t="s">
-        <v>219</v>
-      </c>
-      <c r="K49" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>1994</v>
       </c>
       <c r="B50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C50">
@@ -3720,30 +3522,26 @@
         <v>1.1446165767907364</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
-        <v>1.1446165767907364</v>
-      </c>
-      <c r="H50">
         <f>'Energy data'!K37/'Energy data'!$K$16</f>
         <v>1.6020597233593314</v>
       </c>
-      <c r="I50">
+      <c r="H50">
         <f>'Energy data'!R37/'Energy data'!$R$16</f>
         <v>1.3687143841192309</v>
       </c>
+      <c r="I50" t="s">
+        <v>218</v>
+      </c>
       <c r="J50" t="s">
-        <v>219</v>
-      </c>
-      <c r="K50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>1995</v>
       </c>
       <c r="B51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C51">
@@ -3763,30 +3561,26 @@
         <v>1.1458454489284469</v>
       </c>
       <c r="G51">
-        <f t="shared" si="1"/>
-        <v>1.1458454489284469</v>
-      </c>
-      <c r="H51">
         <f>'Energy data'!K38/'Energy data'!$K$16</f>
         <v>1.7083638557331844</v>
       </c>
-      <c r="I51">
+      <c r="H51">
         <f>'Energy data'!R38/'Energy data'!$R$16</f>
         <v>1.4638361826037947</v>
       </c>
+      <c r="I51" t="s">
+        <v>218</v>
+      </c>
       <c r="J51" t="s">
-        <v>219</v>
-      </c>
-      <c r="K51" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>1996</v>
       </c>
       <c r="B52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C52">
@@ -3806,30 +3600,26 @@
         <v>1.1560121643684795</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
-        <v>1.1560121643684795</v>
-      </c>
-      <c r="H52">
         <f>'Energy data'!K39/'Energy data'!$K$16</f>
         <v>1.7874779161459904</v>
       </c>
-      <c r="I52">
+      <c r="H52">
         <f>'Energy data'!R39/'Energy data'!$R$16</f>
         <v>1.5423633289498402</v>
       </c>
+      <c r="I52" t="s">
+        <v>218</v>
+      </c>
       <c r="J52" t="s">
-        <v>219</v>
-      </c>
-      <c r="K52" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>1997</v>
       </c>
       <c r="B53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C53">
@@ -3849,30 +3639,26 @@
         <v>1.1528869079700799</v>
       </c>
       <c r="G53">
-        <f t="shared" si="1"/>
-        <v>1.1528869079700799</v>
-      </c>
-      <c r="H53">
         <f>'Energy data'!K40/'Energy data'!$K$16</f>
         <v>1.9469987503770414</v>
       </c>
-      <c r="I53">
+      <c r="H53">
         <f>'Energy data'!R40/'Energy data'!$R$16</f>
         <v>1.6019788339908574</v>
       </c>
+      <c r="I53" t="s">
+        <v>218</v>
+      </c>
       <c r="J53" t="s">
-        <v>219</v>
-      </c>
-      <c r="K53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>1998</v>
       </c>
       <c r="B54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C54">
@@ -3892,30 +3678,26 @@
         <v>1.1355485379690513</v>
       </c>
       <c r="G54">
-        <f t="shared" si="1"/>
-        <v>1.1355485379690513</v>
-      </c>
-      <c r="H54">
         <f>'Energy data'!K41/'Energy data'!$K$16</f>
         <v>1.8943422243288659</v>
       </c>
-      <c r="I54">
+      <c r="H54">
         <f>'Energy data'!R41/'Energy data'!$R$16</f>
         <v>1.5893293255682888</v>
       </c>
+      <c r="I54" t="s">
+        <v>218</v>
+      </c>
       <c r="J54" t="s">
-        <v>219</v>
-      </c>
-      <c r="K54" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>1999</v>
       </c>
       <c r="B55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C55">
@@ -3935,30 +3717,26 @@
         <v>1.1294418119467229</v>
       </c>
       <c r="G55">
-        <f t="shared" si="1"/>
-        <v>1.1294418119467229</v>
-      </c>
-      <c r="H55">
         <f>'Energy data'!K42/'Energy data'!$K$16</f>
         <v>1.8629292885767232</v>
       </c>
-      <c r="I55">
+      <c r="H55">
         <f>'Energy data'!R42/'Energy data'!$R$16</f>
         <v>1.5453065314045964</v>
       </c>
+      <c r="I55" t="s">
+        <v>218</v>
+      </c>
       <c r="J55" t="s">
-        <v>219</v>
-      </c>
-      <c r="K55" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>2000</v>
       </c>
       <c r="B56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C56">
@@ -3978,30 +3756,26 @@
         <v>1.1206713526740804</v>
       </c>
       <c r="G56">
-        <f t="shared" si="1"/>
-        <v>1.1206713526740804</v>
-      </c>
-      <c r="H56">
         <f>'Energy data'!K43/'Energy data'!$K$16</f>
         <v>1.9042961175507396</v>
       </c>
-      <c r="I56">
+      <c r="H56">
         <f>'Energy data'!R43/'Energy data'!$R$16</f>
         <v>1.5663472978896613</v>
       </c>
+      <c r="I56" t="s">
+        <v>218</v>
+      </c>
       <c r="J56" t="s">
-        <v>219</v>
-      </c>
-      <c r="K56" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>2001</v>
       </c>
       <c r="B57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C57">
@@ -4021,30 +3795,26 @@
         <v>1.1096287388075015</v>
       </c>
       <c r="G57">
-        <f t="shared" si="1"/>
-        <v>1.1096287388075015</v>
-      </c>
-      <c r="H57">
         <f>'Energy data'!K44/'Energy data'!$K$16</f>
         <v>1.8556470030594225</v>
       </c>
-      <c r="I57">
+      <c r="H57">
         <f>'Energy data'!R44/'Energy data'!$R$16</f>
         <v>1.5470599286116851</v>
       </c>
+      <c r="I57" t="s">
+        <v>218</v>
+      </c>
       <c r="J57" t="s">
-        <v>219</v>
-      </c>
-      <c r="K57" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>2002</v>
       </c>
       <c r="B58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C58">
@@ -4064,30 +3834,26 @@
         <v>1.1549048899999546</v>
       </c>
       <c r="G58">
-        <f t="shared" si="1"/>
-        <v>1.1549048899999546</v>
-      </c>
-      <c r="H58">
         <f>'Energy data'!K45/'Energy data'!$K$16</f>
         <v>1.952859051148361</v>
       </c>
-      <c r="I58">
+      <c r="H58">
         <f>'Energy data'!R45/'Energy data'!$R$16</f>
         <v>1.6297200826601539</v>
       </c>
+      <c r="I58" t="s">
+        <v>218</v>
+      </c>
       <c r="J58" t="s">
-        <v>219</v>
-      </c>
-      <c r="K58" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>2003</v>
       </c>
       <c r="B59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C59">
@@ -4107,30 +3873,26 @@
         <v>1.1445141682138202</v>
       </c>
       <c r="G59">
-        <f t="shared" si="1"/>
-        <v>1.1445141682138202</v>
-      </c>
-      <c r="H59">
         <f>'Energy data'!K46/'Energy data'!$K$16</f>
         <v>1.9979747489981472</v>
       </c>
-      <c r="I59">
+      <c r="H59">
         <f>'Energy data'!R46/'Energy data'!$R$16</f>
         <v>1.6952846139395077</v>
       </c>
+      <c r="I59" t="s">
+        <v>218</v>
+      </c>
       <c r="J59" t="s">
-        <v>219</v>
-      </c>
-      <c r="K59" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>2004</v>
       </c>
       <c r="B60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C60">
@@ -4150,30 +3912,26 @@
         <v>1.152710785725148</v>
       </c>
       <c r="G60">
-        <f t="shared" si="1"/>
-        <v>1.152710785725148</v>
-      </c>
-      <c r="H60">
         <f>'Energy data'!K47/'Energy data'!$K$16</f>
         <v>2.0863101650364113</v>
       </c>
-      <c r="I60">
+      <c r="H60">
         <f>'Energy data'!R47/'Energy data'!$R$16</f>
         <v>1.7300394514371593</v>
       </c>
+      <c r="I60" t="s">
+        <v>218</v>
+      </c>
       <c r="J60" t="s">
-        <v>219</v>
-      </c>
-      <c r="K60" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>2005</v>
       </c>
       <c r="B61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C61">
@@ -4193,30 +3951,26 @@
         <v>1.1489795614486409</v>
       </c>
       <c r="G61">
-        <f t="shared" si="1"/>
-        <v>1.1489795614486409</v>
-      </c>
-      <c r="H61">
         <f>'Energy data'!K48/'Energy data'!$K$16</f>
         <v>2.1118197095703879</v>
       </c>
-      <c r="I61">
+      <c r="H61">
         <f>'Energy data'!R48/'Energy data'!$R$16</f>
         <v>1.7472603168639236</v>
       </c>
+      <c r="I61" t="s">
+        <v>218</v>
+      </c>
       <c r="J61" t="s">
-        <v>219</v>
-      </c>
-      <c r="K61" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>2006</v>
       </c>
       <c r="B62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C62">
@@ -4236,30 +3990,26 @@
         <v>1.1955812540833528</v>
       </c>
       <c r="G62">
-        <f t="shared" si="1"/>
-        <v>1.1955812540833528</v>
-      </c>
-      <c r="H62">
         <f>'Energy data'!K49/'Energy data'!$K$16</f>
         <v>2.0354634377558498</v>
       </c>
-      <c r="I62">
+      <c r="H62">
         <f>'Energy data'!R49/'Energy data'!$R$16</f>
         <v>1.7419375039138327</v>
       </c>
+      <c r="I62" t="s">
+        <v>218</v>
+      </c>
       <c r="J62" t="s">
-        <v>219</v>
-      </c>
-      <c r="K62" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>2007</v>
       </c>
       <c r="B63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C63">
@@ -4279,30 +4029,26 @@
         <v>1.212780495787539</v>
       </c>
       <c r="G63">
-        <f t="shared" si="1"/>
-        <v>1.212780495787539</v>
-      </c>
-      <c r="H63">
         <f>'Energy data'!K50/'Energy data'!$K$16</f>
         <v>2.1911923126642825</v>
       </c>
-      <c r="I63">
+      <c r="H63">
         <f>'Energy data'!R50/'Energy data'!$R$16</f>
         <v>1.9090112092178595</v>
       </c>
+      <c r="I63" t="s">
+        <v>218</v>
+      </c>
       <c r="J63" t="s">
-        <v>219</v>
-      </c>
-      <c r="K63" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>2008</v>
       </c>
       <c r="B64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C64">
@@ -4322,30 +4068,26 @@
         <v>1.2059356699631989</v>
       </c>
       <c r="G64">
-        <f t="shared" si="1"/>
-        <v>1.2059356699631989</v>
-      </c>
-      <c r="H64">
         <f>'Energy data'!K51/'Energy data'!$K$16</f>
         <v>2.3412332485887881</v>
       </c>
-      <c r="I64">
+      <c r="H64">
         <f>'Energy data'!R51/'Energy data'!$R$16</f>
         <v>1.8536539545369148</v>
       </c>
+      <c r="I64" t="s">
+        <v>218</v>
+      </c>
       <c r="J64" t="s">
-        <v>219</v>
-      </c>
-      <c r="K64" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>2009</v>
       </c>
       <c r="B65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C65">
@@ -4365,30 +4107,26 @@
         <v>1.1642851762823798</v>
       </c>
       <c r="G65">
-        <f t="shared" si="1"/>
-        <v>1.1642851762823798</v>
-      </c>
-      <c r="H65">
         <f>'Energy data'!K52/'Energy data'!$K$16</f>
         <v>2.21209117938553</v>
       </c>
-      <c r="I65">
+      <c r="H65">
         <f>'Energy data'!R52/'Energy data'!$R$16</f>
         <v>1.8879704427327944</v>
       </c>
+      <c r="I65" t="s">
+        <v>218</v>
+      </c>
       <c r="J65" t="s">
-        <v>219</v>
-      </c>
-      <c r="K65" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>2010</v>
       </c>
       <c r="B66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C66">
@@ -4408,30 +4146,26 @@
         <v>1.1457617583390758</v>
       </c>
       <c r="G66">
-        <f t="shared" si="1"/>
-        <v>1.1457617583390758</v>
-      </c>
-      <c r="H66">
         <f>'Energy data'!K53/'Energy data'!$K$16</f>
         <v>2.2680225793941484</v>
       </c>
-      <c r="I66">
+      <c r="H66">
         <f>'Energy data'!R53/'Energy data'!$R$16</f>
         <v>1.8787651073955787</v>
       </c>
+      <c r="I66" t="s">
+        <v>218</v>
+      </c>
       <c r="J66" t="s">
-        <v>219</v>
-      </c>
-      <c r="K66" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>2011</v>
       </c>
       <c r="B67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C67">
@@ -4451,30 +4185,26 @@
         <v>1.1603708644982589</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G69" si="3">F67</f>
-        <v>1.1603708644982589</v>
-      </c>
-      <c r="H67">
         <f>'Energy data'!K54/'Energy data'!$K$16</f>
         <v>2.2600077562804324</v>
       </c>
-      <c r="I67">
+      <c r="H67">
         <f>'Energy data'!R54/'Energy data'!$R$16</f>
         <v>1.9590456509487129</v>
       </c>
+      <c r="I67" t="s">
+        <v>218</v>
+      </c>
       <c r="J67" t="s">
-        <v>219</v>
-      </c>
-      <c r="K67" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>2012</v>
       </c>
       <c r="B68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C68">
@@ -4493,29 +4223,25 @@
         <f>'labour '!B75/'labour '!$B$36</f>
         <v>1.1798335520788421</v>
       </c>
-      <c r="G68">
-        <f t="shared" si="3"/>
-        <v>1.1798335520788421</v>
+      <c r="G68" t="s">
+        <v>215</v>
       </c>
       <c r="H68" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I68" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J68" t="s">
-        <v>219</v>
-      </c>
-      <c r="K68" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>2013</v>
       </c>
       <c r="B69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="C69">
@@ -4534,21 +4260,17 @@
         <f>'labour '!B76/'labour '!$B$36</f>
         <v>1.1894539153510799</v>
       </c>
-      <c r="G69">
-        <f t="shared" si="3"/>
-        <v>1.1894539153510799</v>
+      <c r="G69" t="s">
+        <v>215</v>
       </c>
       <c r="H69" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I69" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J69" t="s">
-        <v>219</v>
-      </c>
-      <c r="K69" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>